<commit_message>
update chagne model tables
</commit_message>
<xml_diff>
--- a/Output/Modelling/XGBoost/Tables/change_smote_model_comparison_df.xlsx
+++ b/Output/Modelling/XGBoost/Tables/change_smote_model_comparison_df.xlsx
@@ -467,20 +467,20 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8488</v>
+        <v>0.7415</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.9117</t>
+          <t>0.9118</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.8488</t>
+          <t>0.7415</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0.8787</v>
+        <v>0.8149999999999999</v>
       </c>
     </row>
     <row r="3">
@@ -490,20 +490,20 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9454</v>
+        <v>0.9436</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.9112</t>
+          <t>0.9120</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.9454</t>
+          <t>0.9436</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.928</v>
+        <v>0.9276</v>
       </c>
     </row>
     <row r="4">

</xml_diff>